<commit_message>
fix ids in 2.0.0 requirement set
</commit_message>
<xml_diff>
--- a/lib/smart_app_launch/requirements/hl7.fhir.uv.smart-app-launch_2.0.0_Requirements.xlsx
+++ b/lib/smart_app_launch/requirements/hl7.fhir.uv.smart-app-launch_2.0.0_Requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/knaden/Documents/Inferno/source/smart-app-launch-test-kit/lib/smart_app_launch/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFD23E3-4A35-9245-A61F-6B87660479BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A796EA-224D-5C41-A142-7EC2648B7A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="31820" windowHeight="16620" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -3836,6 +3836,21 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3853,21 +3868,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4239,14 +4239,14 @@
       <c r="C3" s="22"/>
     </row>
     <row r="4" spans="1:3" ht="409.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="47" t="s">
         <v>587</v>
       </c>
       <c r="B4" s="23"/>
       <c r="C4" s="24"/>
     </row>
     <row r="5" spans="1:3" ht="258" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="43"/>
+      <c r="A5" s="48"/>
       <c r="B5" s="27"/>
       <c r="C5" s="22"/>
     </row>
@@ -4258,17 +4258,17 @@
       <c r="C6" s="17"/>
     </row>
     <row r="7" spans="1:3" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="45"/>
+      <c r="B7" s="50"/>
     </row>
     <row r="8" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="44"/>
-      <c r="B8" s="46"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="51"/>
     </row>
     <row r="9" spans="1:3" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="42"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="26"/>
     </row>
     <row r="10" spans="1:3" ht="292" x14ac:dyDescent="0.2">
@@ -4294,10 +4294,10 @@
   <dimension ref="A1:AC493"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G437" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G394" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A439" sqref="A439:XFD440"/>
+      <selection pane="bottomRight" activeCell="A265" sqref="A265:A269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5099,7 +5099,7 @@
     </row>
     <row r="25" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="37">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="35" t="s">
         <v>535</v>
@@ -5116,7 +5116,7 @@
     </row>
     <row r="26" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A26" s="37">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B26" s="35" t="s">
         <v>532</v>
@@ -5144,7 +5144,7 @@
     </row>
     <row r="27" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A27" s="37">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B27" s="35" t="s">
         <v>532</v>
@@ -5172,7 +5172,7 @@
     </row>
     <row r="28" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A28" s="37">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B28" s="35" t="s">
         <v>532</v>
@@ -5200,7 +5200,7 @@
     </row>
     <row r="29" spans="1:20" ht="136" x14ac:dyDescent="0.2">
       <c r="A29" s="37">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B29" s="35" t="s">
         <v>532</v>
@@ -5228,7 +5228,7 @@
     </row>
     <row r="30" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A30" s="37">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B30" s="35" t="s">
         <v>536</v>
@@ -5245,7 +5245,7 @@
     </row>
     <row r="31" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" s="37">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B31" s="35" t="s">
         <v>537</v>
@@ -5270,7 +5270,7 @@
     </row>
     <row r="32" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A32" s="37">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B32" s="35" t="s">
         <v>538</v>
@@ -5295,7 +5295,7 @@
     </row>
     <row r="33" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A33" s="37">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B33" s="35" t="s">
         <v>538</v>
@@ -5320,7 +5320,7 @@
     </row>
     <row r="34" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="37">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B34" s="35" t="s">
         <v>538</v>
@@ -5345,7 +5345,7 @@
     </row>
     <row r="35" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" s="37">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B35" s="35" t="s">
         <v>538</v>
@@ -5370,7 +5370,7 @@
     </row>
     <row r="36" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A36" s="37">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B36" s="35" t="s">
         <v>538</v>
@@ -5395,7 +5395,7 @@
     </row>
     <row r="37" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="37">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B37" s="35" t="s">
         <v>538</v>
@@ -5420,7 +5420,7 @@
     </row>
     <row r="38" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A38" s="37">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B38" s="35" t="s">
         <v>538</v>
@@ -5448,7 +5448,7 @@
     </row>
     <row r="39" spans="1:20" ht="153" x14ac:dyDescent="0.2">
       <c r="A39" s="37">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B39" s="35" t="s">
         <v>538</v>
@@ -5476,7 +5476,7 @@
     </row>
     <row r="40" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A40" s="37">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B40" s="35" t="s">
         <v>538</v>
@@ -5501,7 +5501,7 @@
     </row>
     <row r="41" spans="1:20" ht="136" x14ac:dyDescent="0.2">
       <c r="A41" s="37">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B41" s="35" t="s">
         <v>538</v>
@@ -5526,7 +5526,7 @@
     </row>
     <row r="42" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A42" s="37">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B42" s="35" t="s">
         <v>538</v>
@@ -5551,7 +5551,7 @@
     </row>
     <row r="43" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="37">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B43" s="35" t="s">
         <v>538</v>
@@ -5576,7 +5576,7 @@
     </row>
     <row r="44" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="37">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B44" s="35" t="s">
         <v>538</v>
@@ -5601,7 +5601,7 @@
     </row>
     <row r="45" spans="1:20" ht="153" x14ac:dyDescent="0.2">
       <c r="A45" s="37">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B45" s="35" t="s">
         <v>538</v>
@@ -5626,7 +5626,7 @@
     </row>
     <row r="46" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A46" s="37">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B46" s="35" t="s">
         <v>538</v>
@@ -5651,7 +5651,7 @@
     </row>
     <row r="47" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A47" s="37">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B47" s="35" t="s">
         <v>538</v>
@@ -5676,7 +5676,7 @@
     </row>
     <row r="48" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A48" s="37">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B48" s="35" t="s">
         <v>538</v>
@@ -5701,7 +5701,7 @@
     </row>
     <row r="49" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A49" s="37">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B49" s="35" t="s">
         <v>538</v>
@@ -5726,7 +5726,7 @@
     </row>
     <row r="50" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A50" s="37">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="B50" s="35" t="s">
         <v>538</v>
@@ -5751,7 +5751,7 @@
     </row>
     <row r="51" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A51" s="37">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B51" s="35" t="s">
         <v>538</v>
@@ -5776,7 +5776,7 @@
     </row>
     <row r="52" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A52" s="37">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B52" s="35" t="s">
         <v>538</v>
@@ -5801,7 +5801,7 @@
     </row>
     <row r="53" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A53" s="37">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B53" s="35" t="s">
         <v>538</v>
@@ -5826,7 +5826,7 @@
     </row>
     <row r="54" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A54" s="37">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="B54" s="35" t="s">
         <v>542</v>
@@ -5843,7 +5843,7 @@
     </row>
     <row r="55" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A55" s="37">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B55" s="35" t="s">
         <v>542</v>
@@ -5868,7 +5868,7 @@
     </row>
     <row r="56" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A56" s="37">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B56" s="35" t="s">
         <v>542</v>
@@ -5888,7 +5888,7 @@
     </row>
     <row r="57" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A57" s="37">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B57" s="35" t="s">
         <v>542</v>
@@ -5913,7 +5913,7 @@
     </row>
     <row r="58" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A58" s="37">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="B58" s="35" t="s">
         <v>542</v>
@@ -5938,7 +5938,7 @@
     </row>
     <row r="59" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A59" s="37">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="B59" s="35" t="s">
         <v>542</v>
@@ -5963,7 +5963,7 @@
     </row>
     <row r="60" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A60" s="37">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B60" s="35" t="s">
         <v>542</v>
@@ -5988,7 +5988,7 @@
     </row>
     <row r="61" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A61" s="37">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="B61" s="35" t="s">
         <v>542</v>
@@ -6013,7 +6013,7 @@
     </row>
     <row r="62" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A62" s="37">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="B62" s="35" t="s">
         <v>542</v>
@@ -6038,7 +6038,7 @@
     </row>
     <row r="63" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A63" s="37">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="B63" s="35" t="s">
         <v>539</v>
@@ -6063,7 +6063,7 @@
     </row>
     <row r="64" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A64" s="37">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>539</v>
@@ -6088,7 +6088,7 @@
     </row>
     <row r="65" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A65" s="37">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>539</v>
@@ -6113,7 +6113,7 @@
     </row>
     <row r="66" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A66" s="37">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>539</v>
@@ -6130,7 +6130,7 @@
     </row>
     <row r="67" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A67" s="37">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="B67" s="35" t="s">
         <v>539</v>
@@ -6155,7 +6155,7 @@
     </row>
     <row r="68" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A68" s="37">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>539</v>
@@ -6180,7 +6180,7 @@
     </row>
     <row r="69" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A69" s="37">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="B69" s="35" t="s">
         <v>539</v>
@@ -6205,7 +6205,7 @@
     </row>
     <row r="70" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A70" s="37">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="B70" s="35" t="s">
         <v>539</v>
@@ -6230,7 +6230,7 @@
     </row>
     <row r="71" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A71" s="37">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B71" s="35" t="s">
         <v>539</v>
@@ -6255,7 +6255,7 @@
     </row>
     <row r="72" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A72" s="37">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="B72" s="35" t="s">
         <v>539</v>
@@ -6280,7 +6280,7 @@
     </row>
     <row r="73" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" s="37">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="B73" s="35" t="s">
         <v>539</v>
@@ -6305,7 +6305,7 @@
     </row>
     <row r="74" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A74" s="37">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>544</v>
@@ -6330,7 +6330,7 @@
     </row>
     <row r="75" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A75" s="37">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>544</v>
@@ -6355,7 +6355,7 @@
     </row>
     <row r="76" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A76" s="37">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>544</v>
@@ -6380,7 +6380,7 @@
     </row>
     <row r="77" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A77" s="37">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>544</v>
@@ -6405,7 +6405,7 @@
     </row>
     <row r="78" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A78" s="37">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>544</v>
@@ -6430,7 +6430,7 @@
     </row>
     <row r="79" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A79" s="37">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>544</v>
@@ -6455,7 +6455,7 @@
     </row>
     <row r="80" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A80" s="37">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>544</v>
@@ -6480,7 +6480,7 @@
     </row>
     <row r="81" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A81" s="37">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>544</v>
@@ -6505,7 +6505,7 @@
     </row>
     <row r="82" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A82" s="37">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>544</v>
@@ -6530,7 +6530,7 @@
     </row>
     <row r="83" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A83" s="37">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>544</v>
@@ -6555,7 +6555,7 @@
     </row>
     <row r="84" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A84" s="37">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>544</v>
@@ -6580,7 +6580,7 @@
     </row>
     <row r="85" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A85" s="37">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>544</v>
@@ -6605,7 +6605,7 @@
     </row>
     <row r="86" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A86" s="37">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>544</v>
@@ -6622,7 +6622,7 @@
     </row>
     <row r="87" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A87" s="37">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>544</v>
@@ -6647,7 +6647,7 @@
     </row>
     <row r="88" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A88" s="37">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>544</v>
@@ -6672,7 +6672,7 @@
     </row>
     <row r="89" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A89" s="37">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>544</v>
@@ -6690,7 +6690,7 @@
     </row>
     <row r="90" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A90" s="37">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>544</v>
@@ -6708,7 +6708,7 @@
     </row>
     <row r="91" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A91" s="37">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>544</v>
@@ -6733,7 +6733,7 @@
     </row>
     <row r="92" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A92" s="37">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>544</v>
@@ -6758,7 +6758,7 @@
     </row>
     <row r="93" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A93" s="37">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="B93" s="35" t="s">
         <v>107</v>
@@ -6783,7 +6783,7 @@
     </row>
     <row r="94" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A94" s="37">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="B94" s="35" t="s">
         <v>540</v>
@@ -6800,7 +6800,7 @@
     </row>
     <row r="95" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A95" s="37">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="B95" s="35" t="s">
         <v>545</v>
@@ -6825,7 +6825,7 @@
     </row>
     <row r="96" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A96" s="37">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="B96" s="35" t="s">
         <v>545</v>
@@ -6850,7 +6850,7 @@
     </row>
     <row r="97" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A97" s="37">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="B97" s="35" t="s">
         <v>545</v>
@@ -6867,7 +6867,7 @@
     </row>
     <row r="98" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A98" s="37">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="B98" s="35" t="s">
         <v>545</v>
@@ -6892,7 +6892,7 @@
     </row>
     <row r="99" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A99" s="37">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="B99" s="35" t="s">
         <v>545</v>
@@ -6917,7 +6917,7 @@
     </row>
     <row r="100" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A100" s="37">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="B100" s="35" t="s">
         <v>546</v>
@@ -6942,7 +6942,7 @@
     </row>
     <row r="101" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A101" s="37">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="B101" s="35" t="s">
         <v>546</v>
@@ -6970,7 +6970,7 @@
     </row>
     <row r="102" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A102" s="37">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="B102" s="35" t="s">
         <v>546</v>
@@ -6998,7 +6998,7 @@
     </row>
     <row r="103" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A103" s="37">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="B103" s="35" t="s">
         <v>546</v>
@@ -7015,7 +7015,7 @@
     </row>
     <row r="104" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A104" s="37">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="B104" s="35" t="s">
         <v>546</v>
@@ -7040,7 +7040,7 @@
     </row>
     <row r="105" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A105" s="37">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="B105" s="35" t="s">
         <v>546</v>
@@ -7065,7 +7065,7 @@
     </row>
     <row r="106" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A106" s="37">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="B106" s="35" t="s">
         <v>541</v>
@@ -7090,7 +7090,7 @@
     </row>
     <row r="107" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A107" s="37">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="B107" s="35" t="s">
         <v>541</v>
@@ -7115,7 +7115,7 @@
     </row>
     <row r="108" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A108" s="37">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="B108" s="35" t="s">
         <v>541</v>
@@ -7140,7 +7140,7 @@
     </row>
     <row r="109" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A109" s="37">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="B109" s="35" t="s">
         <v>541</v>
@@ -7165,7 +7165,7 @@
     </row>
     <row r="110" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A110" s="37">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="B110" s="35" t="s">
         <v>541</v>
@@ -7193,7 +7193,7 @@
     </row>
     <row r="111" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A111" s="37">
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="B111" s="35" t="s">
         <v>547</v>
@@ -7218,7 +7218,7 @@
     </row>
     <row r="112" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A112" s="37">
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="B112" s="35" t="s">
         <v>547</v>
@@ -7243,7 +7243,7 @@
     </row>
     <row r="113" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A113" s="37">
-        <v>32</v>
+        <v>112</v>
       </c>
       <c r="B113" s="35" t="s">
         <v>547</v>
@@ -7268,7 +7268,7 @@
     </row>
     <row r="114" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A114" s="37">
-        <v>32</v>
+        <v>113</v>
       </c>
       <c r="B114" s="35" t="s">
         <v>547</v>
@@ -7293,7 +7293,7 @@
     </row>
     <row r="115" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A115" s="37">
-        <v>32</v>
+        <v>114</v>
       </c>
       <c r="B115" s="35" t="s">
         <v>547</v>
@@ -7318,7 +7318,7 @@
     </row>
     <row r="116" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A116" s="37">
-        <v>32</v>
+        <v>115</v>
       </c>
       <c r="B116" s="35" t="s">
         <v>547</v>
@@ -7343,7 +7343,7 @@
     </row>
     <row r="117" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A117" s="37">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="B117" s="35" t="s">
         <v>547</v>
@@ -7368,7 +7368,7 @@
     </row>
     <row r="118" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A118" s="37">
-        <v>32</v>
+        <v>117</v>
       </c>
       <c r="B118" s="35" t="s">
         <v>547</v>
@@ -7393,7 +7393,7 @@
     </row>
     <row r="119" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A119" s="37">
-        <v>32</v>
+        <v>118</v>
       </c>
       <c r="B119" s="35" t="s">
         <v>547</v>
@@ -7418,7 +7418,7 @@
     </row>
     <row r="120" spans="1:14" ht="80" x14ac:dyDescent="0.2">
       <c r="A120" s="37">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="B120" s="35" t="s">
         <v>549</v>
@@ -7435,7 +7435,7 @@
     </row>
     <row r="121" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A121" s="37">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="B121" s="35" t="s">
         <v>550</v>
@@ -7460,7 +7460,7 @@
     </row>
     <row r="122" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A122" s="37">
-        <v>32</v>
+        <v>121</v>
       </c>
       <c r="B122" s="35" t="s">
         <v>550</v>
@@ -7485,7 +7485,7 @@
     </row>
     <row r="123" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A123" s="37">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="B123" s="35" t="s">
         <v>550</v>
@@ -7510,7 +7510,7 @@
     </row>
     <row r="124" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A124" s="37">
-        <v>32</v>
+        <v>123</v>
       </c>
       <c r="B124" s="35" t="s">
         <v>550</v>
@@ -7527,7 +7527,7 @@
     </row>
     <row r="125" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A125" s="37">
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="B125" s="35" t="s">
         <v>550</v>
@@ -7552,7 +7552,7 @@
     </row>
     <row r="126" spans="1:14" ht="136" x14ac:dyDescent="0.2">
       <c r="A126" s="37">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="B126" s="35" t="s">
         <v>550</v>
@@ -7577,7 +7577,7 @@
     </row>
     <row r="127" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A127" s="37">
-        <v>32</v>
+        <v>126</v>
       </c>
       <c r="B127" s="35" t="s">
         <v>550</v>
@@ -7602,7 +7602,7 @@
     </row>
     <row r="128" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A128" s="37">
-        <v>32</v>
+        <v>127</v>
       </c>
       <c r="B128" s="35" t="s">
         <v>550</v>
@@ -7627,7 +7627,7 @@
     </row>
     <row r="129" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A129" s="37">
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="B129" s="35" t="s">
         <v>550</v>
@@ -7652,7 +7652,7 @@
     </row>
     <row r="130" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A130" s="37">
-        <v>32</v>
+        <v>129</v>
       </c>
       <c r="B130" s="35" t="s">
         <v>550</v>
@@ -7677,7 +7677,7 @@
     </row>
     <row r="131" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A131" s="37">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="B131" s="35" t="s">
         <v>551</v>
@@ -7697,7 +7697,7 @@
     </row>
     <row r="132" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A132" s="37">
-        <v>32</v>
+        <v>131</v>
       </c>
       <c r="B132" s="35" t="s">
         <v>553</v>
@@ -7722,7 +7722,7 @@
     </row>
     <row r="133" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A133" s="37">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="B133" s="35" t="s">
         <v>554</v>
@@ -7742,7 +7742,7 @@
     </row>
     <row r="134" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A134" s="37">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="B134" s="35" t="s">
         <v>555</v>
@@ -7759,7 +7759,7 @@
     </row>
     <row r="135" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A135" s="37">
-        <v>32</v>
+        <v>134</v>
       </c>
       <c r="B135" s="35" t="s">
         <v>555</v>
@@ -7776,7 +7776,7 @@
     </row>
     <row r="136" spans="1:20" ht="255" x14ac:dyDescent="0.2">
       <c r="A136" s="37">
-        <v>32</v>
+        <v>135</v>
       </c>
       <c r="B136" s="35" t="s">
         <v>556</v>
@@ -7796,7 +7796,7 @@
     </row>
     <row r="137" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A137" s="37">
-        <v>32</v>
+        <v>136</v>
       </c>
       <c r="B137" s="35" t="s">
         <v>557</v>
@@ -7813,7 +7813,7 @@
     </row>
     <row r="138" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A138" s="37">
-        <v>32</v>
+        <v>137</v>
       </c>
       <c r="B138" s="35" t="s">
         <v>557</v>
@@ -7830,7 +7830,7 @@
     </row>
     <row r="139" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A139" s="37">
-        <v>32</v>
+        <v>138</v>
       </c>
       <c r="B139" s="35" t="s">
         <v>557</v>
@@ -7847,7 +7847,7 @@
     </row>
     <row r="140" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A140" s="37">
-        <v>32</v>
+        <v>139</v>
       </c>
       <c r="B140" s="35" t="s">
         <v>557</v>
@@ -7872,7 +7872,7 @@
     </row>
     <row r="141" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A141" s="37">
-        <v>32</v>
+        <v>140</v>
       </c>
       <c r="B141" s="35" t="s">
         <v>558</v>
@@ -7889,7 +7889,7 @@
     </row>
     <row r="142" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A142" s="37">
-        <v>32</v>
+        <v>141</v>
       </c>
       <c r="B142" s="35" t="s">
         <v>558</v>
@@ -7906,7 +7906,7 @@
     </row>
     <row r="143" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A143" s="37">
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="B143" s="35" t="s">
         <v>559</v>
@@ -7923,7 +7923,7 @@
     </row>
     <row r="144" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A144" s="37">
-        <v>32</v>
+        <v>143</v>
       </c>
       <c r="B144" s="35" t="s">
         <v>559</v>
@@ -7940,7 +7940,7 @@
     </row>
     <row r="145" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A145" s="37">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="B145" s="35" t="s">
         <v>560</v>
@@ -7957,7 +7957,7 @@
     </row>
     <row r="146" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A146" s="37">
-        <v>32</v>
+        <v>145</v>
       </c>
       <c r="B146" s="35" t="s">
         <v>560</v>
@@ -7974,7 +7974,7 @@
     </row>
     <row r="147" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A147" s="37">
-        <v>32</v>
+        <v>146</v>
       </c>
       <c r="B147" s="35" t="s">
         <v>560</v>
@@ -7991,7 +7991,7 @@
     </row>
     <row r="148" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A148" s="37">
-        <v>32</v>
+        <v>147</v>
       </c>
       <c r="B148" s="35" t="s">
         <v>560</v>
@@ -8008,7 +8008,7 @@
     </row>
     <row r="149" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A149" s="37">
-        <v>32</v>
+        <v>148</v>
       </c>
       <c r="B149" s="35" t="s">
         <v>560</v>
@@ -8033,7 +8033,7 @@
     </row>
     <row r="150" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A150" s="37">
-        <v>32</v>
+        <v>149</v>
       </c>
       <c r="B150" s="35" t="s">
         <v>561</v>
@@ -8050,7 +8050,7 @@
     </row>
     <row r="151" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A151" s="37">
-        <v>32</v>
+        <v>150</v>
       </c>
       <c r="B151" s="35" t="s">
         <v>561</v>
@@ -8067,7 +8067,7 @@
     </row>
     <row r="152" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A152" s="37">
-        <v>32</v>
+        <v>151</v>
       </c>
       <c r="B152" s="35" t="s">
         <v>561</v>
@@ -8084,7 +8084,7 @@
     </row>
     <row r="153" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A153" s="37">
-        <v>32</v>
+        <v>152</v>
       </c>
       <c r="B153" s="35" t="s">
         <v>563</v>
@@ -8101,7 +8101,7 @@
     </row>
     <row r="154" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A154" s="37">
-        <v>32</v>
+        <v>153</v>
       </c>
       <c r="B154" s="35" t="s">
         <v>563</v>
@@ -8318,7 +8318,7 @@
     </row>
     <row r="163" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A163" s="37">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B163" s="35" t="s">
         <v>562</v>
@@ -8343,7 +8343,7 @@
     </row>
     <row r="164" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A164" s="37">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B164" s="35" t="s">
         <v>562</v>
@@ -8368,7 +8368,7 @@
     </row>
     <row r="165" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A165" s="37">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B165" s="35" t="s">
         <v>562</v>
@@ -8393,7 +8393,7 @@
     </row>
     <row r="166" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A166" s="37">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B166" s="35" t="s">
         <v>562</v>
@@ -8418,7 +8418,7 @@
     </row>
     <row r="167" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A167" s="37">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B167" s="35" t="s">
         <v>563</v>
@@ -8443,7 +8443,7 @@
     </row>
     <row r="168" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A168" s="37">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B168" s="35" t="s">
         <v>563</v>
@@ -8468,7 +8468,7 @@
     </row>
     <row r="169" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A169" s="37">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B169" s="35" t="s">
         <v>564</v>
@@ -8493,7 +8493,7 @@
     </row>
     <row r="170" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A170" s="37">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B170" s="35" t="s">
         <v>564</v>
@@ -8510,7 +8510,7 @@
     </row>
     <row r="171" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A171" s="37">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B171" s="35" t="s">
         <v>564</v>
@@ -8527,7 +8527,7 @@
     </row>
     <row r="172" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A172" s="37">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="B172" s="35" t="s">
         <v>564</v>
@@ -8544,7 +8544,7 @@
     </row>
     <row r="173" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A173" s="37">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="B173" s="35" t="s">
         <v>564</v>
@@ -8561,7 +8561,7 @@
     </row>
     <row r="174" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A174" s="37">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="B174" s="35" t="s">
         <v>564</v>
@@ -8578,7 +8578,7 @@
     </row>
     <row r="175" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A175" s="37">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="B175" s="35" t="s">
         <v>564</v>
@@ -8595,7 +8595,7 @@
     </row>
     <row r="176" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A176" s="37">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="B176" s="35" t="s">
         <v>564</v>
@@ -8612,7 +8612,7 @@
     </row>
     <row r="177" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A177" s="37">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="B177" s="35" t="s">
         <v>564</v>
@@ -8643,7 +8643,7 @@
       <c r="E178" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="T178" s="48" t="s">
+      <c r="T178" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -8663,7 +8663,7 @@
       <c r="E179" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="T179" s="48" t="s">
+      <c r="T179" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -8683,7 +8683,7 @@
       <c r="E180" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="T180" s="48" t="s">
+      <c r="T180" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -8703,7 +8703,7 @@
       <c r="E181" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="T181" s="48" t="s">
+      <c r="T181" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -8723,7 +8723,7 @@
       <c r="E182" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="T182" s="48" t="s">
+      <c r="T182" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -8743,7 +8743,7 @@
       <c r="E183" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="T183" s="48" t="s">
+      <c r="T183" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -8763,7 +8763,7 @@
       <c r="E184" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="T184" s="48" t="s">
+      <c r="T184" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -8783,7 +8783,7 @@
       <c r="E185" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="T185" s="48" t="s">
+      <c r="T185" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -8803,7 +8803,7 @@
       <c r="E186" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="T186" s="48" t="s">
+      <c r="T186" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -8823,7 +8823,7 @@
       <c r="E187" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="T187" s="48" t="s">
+      <c r="T187" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -8843,7 +8843,7 @@
       <c r="E188" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="T188" s="48" t="s">
+      <c r="T188" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -8863,7 +8863,7 @@
       <c r="E189" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="T189" s="48" t="s">
+      <c r="T189" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -8883,7 +8883,7 @@
       <c r="E190" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="T190" s="48" t="s">
+      <c r="T190" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -8903,7 +8903,7 @@
       <c r="E191" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="T191" s="48" t="s">
+      <c r="T191" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -8923,7 +8923,7 @@
       <c r="E192" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="T192" s="48" t="s">
+      <c r="T192" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -8943,7 +8943,7 @@
       <c r="E193" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="T193" s="48" t="s">
+      <c r="T193" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -8974,7 +8974,7 @@
     </row>
     <row r="195" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A195" s="37">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B195" s="35" t="s">
         <v>565</v>
@@ -8991,7 +8991,7 @@
     </row>
     <row r="196" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A196" s="37">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B196" s="35" t="s">
         <v>566</v>
@@ -9016,7 +9016,7 @@
     </row>
     <row r="197" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A197" s="37">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B197" s="35" t="s">
         <v>566</v>
@@ -9058,7 +9058,7 @@
         <f t="array" ref="N198">SECTION_NAME(B198)</f>
         <v>scopes-for-requesting-identity-data</v>
       </c>
-      <c r="T198" s="48" t="s">
+      <c r="T198" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -9081,7 +9081,7 @@
     </row>
     <row r="200" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A200" s="37">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B200" s="35" t="s">
         <v>566</v>
@@ -9098,7 +9098,7 @@
     </row>
     <row r="201" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A201" s="37">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B201" s="35" t="s">
         <v>566</v>
@@ -9123,7 +9123,7 @@
     </row>
     <row r="202" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A202" s="37">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B202" s="35" t="s">
         <v>566</v>
@@ -9140,7 +9140,7 @@
     </row>
     <row r="203" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A203" s="37">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B203" s="35" t="s">
         <v>566</v>
@@ -9168,7 +9168,7 @@
     </row>
     <row r="204" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A204" s="37">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="B204" s="35" t="s">
         <v>566</v>
@@ -9193,7 +9193,7 @@
     </row>
     <row r="205" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A205" s="37">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B205" s="35" t="s">
         <v>566</v>
@@ -9218,7 +9218,7 @@
     </row>
     <row r="206" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A206" s="37">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="B206" s="35" t="s">
         <v>566</v>
@@ -9243,7 +9243,7 @@
     </row>
     <row r="207" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A207" s="37">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B207" s="35" t="s">
         <v>566</v>
@@ -9268,7 +9268,7 @@
     </row>
     <row r="208" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A208" s="37">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="B208" s="35" t="s">
         <v>566</v>
@@ -9293,7 +9293,7 @@
     </row>
     <row r="209" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A209" s="37">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="B209" s="35" t="s">
         <v>566</v>
@@ -9310,7 +9310,7 @@
     </row>
     <row r="210" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A210" s="37">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="B210" s="35" t="s">
         <v>566</v>
@@ -9335,7 +9335,7 @@
     </row>
     <row r="211" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A211" s="37">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="B211" s="35" t="s">
         <v>566</v>
@@ -9360,7 +9360,7 @@
     </row>
     <row r="212" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A212" s="37">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="B212" s="35" t="s">
         <v>566</v>
@@ -9385,7 +9385,7 @@
     </row>
     <row r="213" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A213" s="37">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="B213" s="35" t="s">
         <v>566</v>
@@ -9410,7 +9410,7 @@
     </row>
     <row r="214" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A214" s="37">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="B214" s="35" t="s">
         <v>566</v>
@@ -9435,7 +9435,7 @@
     </row>
     <row r="215" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A215" s="37">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="B215" s="35" t="s">
         <v>566</v>
@@ -9460,7 +9460,7 @@
     </row>
     <row r="216" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A216" s="37">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="B216" s="35" t="s">
         <v>567</v>
@@ -9485,7 +9485,7 @@
     </row>
     <row r="217" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A217" s="37">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="B217" s="35" t="s">
         <v>567</v>
@@ -9510,7 +9510,7 @@
     </row>
     <row r="218" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A218" s="37">
-        <v>198</v>
+        <v>217</v>
       </c>
       <c r="B218" s="35" t="s">
         <v>568</v>
@@ -9527,7 +9527,7 @@
     </row>
     <row r="219" spans="1:20" ht="204" x14ac:dyDescent="0.2">
       <c r="A219" s="37">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="B219" s="35" t="s">
         <v>569</v>
@@ -9602,7 +9602,7 @@
     </row>
     <row r="222" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A222" s="37">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B222" s="35" t="s">
         <v>571</v>
@@ -9630,7 +9630,7 @@
     </row>
     <row r="223" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A223" s="37">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B223" s="35" t="s">
         <v>571</v>
@@ -9658,7 +9658,7 @@
     </row>
     <row r="224" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A224" s="37">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B224" s="35" t="s">
         <v>571</v>
@@ -9686,7 +9686,7 @@
     </row>
     <row r="225" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A225" s="37">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B225" s="35" t="s">
         <v>571</v>
@@ -9714,7 +9714,7 @@
     </row>
     <row r="226" spans="1:20" ht="136" x14ac:dyDescent="0.2">
       <c r="A226" s="37">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="B226" s="35" t="s">
         <v>572</v>
@@ -9739,7 +9739,7 @@
     </row>
     <row r="227" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A227" s="37">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B227" s="35" t="s">
         <v>573</v>
@@ -9764,7 +9764,7 @@
     </row>
     <row r="228" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A228" s="37">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="B228" s="35" t="s">
         <v>574</v>
@@ -9789,7 +9789,7 @@
     </row>
     <row r="229" spans="1:20" ht="136" x14ac:dyDescent="0.2">
       <c r="A229" s="37">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B229" s="35" t="s">
         <v>575</v>
@@ -9814,7 +9814,7 @@
     </row>
     <row r="230" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A230" s="37">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="B230" s="35" t="s">
         <v>576</v>
@@ -9839,7 +9839,7 @@
     </row>
     <row r="231" spans="1:20" ht="136" x14ac:dyDescent="0.2">
       <c r="A231" s="37">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="B231" s="35" t="s">
         <v>577</v>
@@ -9864,7 +9864,7 @@
     </row>
     <row r="232" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A232" s="37">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="B232" s="35" t="s">
         <v>577</v>
@@ -9889,7 +9889,7 @@
     </row>
     <row r="233" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A233" s="37">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="B233" s="35" t="s">
         <v>577</v>
@@ -9914,7 +9914,7 @@
     </row>
     <row r="234" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A234" s="37">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="B234" s="35" t="s">
         <v>577</v>
@@ -9939,7 +9939,7 @@
     </row>
     <row r="235" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A235" s="37">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="B235" s="35" t="s">
         <v>577</v>
@@ -9964,7 +9964,7 @@
     </row>
     <row r="236" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A236" s="37">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="B236" s="35" t="s">
         <v>577</v>
@@ -9989,7 +9989,7 @@
     </row>
     <row r="237" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A237" s="37">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="B237" s="35" t="s">
         <v>577</v>
@@ -10014,7 +10014,7 @@
     </row>
     <row r="238" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A238" s="37">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="B238" s="35" t="s">
         <v>577</v>
@@ -10039,7 +10039,7 @@
     </row>
     <row r="239" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A239" s="37">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="B239" s="35" t="s">
         <v>577</v>
@@ -10064,7 +10064,7 @@
     </row>
     <row r="240" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A240" s="37">
-        <v>221</v>
+        <v>239</v>
       </c>
       <c r="B240" s="35" t="s">
         <v>579</v>
@@ -10079,23 +10079,23 @@
         <v>28</v>
       </c>
     </row>
-    <row r="241" spans="1:20" s="49" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A241" s="49">
+    <row r="241" spans="1:20" s="43" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A241" s="43">
         <v>240</v>
       </c>
-      <c r="B241" s="50" t="s">
+      <c r="B241" s="44" t="s">
         <v>579</v>
       </c>
-      <c r="C241" s="51" t="s">
+      <c r="C241" s="45" t="s">
         <v>590</v>
       </c>
-      <c r="D241" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="E241" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="T241" s="52" t="s">
+      <c r="D241" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="E241" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="T241" s="46" t="s">
         <v>591</v>
       </c>
     </row>
@@ -10135,7 +10135,7 @@
     </row>
     <row r="244" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A244" s="37">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B244" s="35" t="s">
         <v>581</v>
@@ -10160,7 +10160,7 @@
     </row>
     <row r="245" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A245" s="37">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B245" s="35" t="s">
         <v>581</v>
@@ -10185,7 +10185,7 @@
     </row>
     <row r="246" spans="1:20" ht="153" x14ac:dyDescent="0.2">
       <c r="A246" s="37">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B246" s="35" t="s">
         <v>581</v>
@@ -10210,7 +10210,7 @@
     </row>
     <row r="247" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A247" s="37">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B247" s="35" t="s">
         <v>581</v>
@@ -10235,7 +10235,7 @@
     </row>
     <row r="248" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A248" s="37">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B248" s="35" t="s">
         <v>581</v>
@@ -10260,7 +10260,7 @@
     </row>
     <row r="249" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A249" s="37">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B249" s="35" t="s">
         <v>581</v>
@@ -10277,7 +10277,7 @@
     </row>
     <row r="250" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A250" s="37">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="B250" s="35" t="s">
         <v>582</v>
@@ -10294,7 +10294,7 @@
     </row>
     <row r="251" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A251" s="37">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="B251" s="35" t="s">
         <v>583</v>
@@ -10319,7 +10319,7 @@
     </row>
     <row r="252" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A252" s="37">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="B252" s="35" t="s">
         <v>584</v>
@@ -10344,7 +10344,7 @@
     </row>
     <row r="253" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A253" s="37">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="B253" s="35" t="s">
         <v>584</v>
@@ -10369,7 +10369,7 @@
     </row>
     <row r="254" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A254" s="37">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="B254" s="35" t="s">
         <v>584</v>
@@ -10394,7 +10394,7 @@
     </row>
     <row r="255" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A255" s="37">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="B255" s="35" t="s">
         <v>584</v>
@@ -10419,7 +10419,7 @@
     </row>
     <row r="256" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A256" s="37">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="B256" s="35" t="s">
         <v>584</v>
@@ -10444,7 +10444,7 @@
     </row>
     <row r="257" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A257" s="37">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="B257" s="35" t="s">
         <v>584</v>
@@ -10469,7 +10469,7 @@
     </row>
     <row r="258" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A258" s="37">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="B258" s="35" t="s">
         <v>584</v>
@@ -10494,7 +10494,7 @@
     </row>
     <row r="259" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A259" s="37">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="B259" s="35" t="s">
         <v>584</v>
@@ -10519,7 +10519,7 @@
     </row>
     <row r="260" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A260" s="37">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="B260" s="35" t="s">
         <v>584</v>
@@ -10544,7 +10544,7 @@
     </row>
     <row r="261" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A261" s="37">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="B261" s="35" t="s">
         <v>584</v>
@@ -10569,7 +10569,7 @@
     </row>
     <row r="262" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A262" s="37">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="B262" s="35" t="s">
         <v>584</v>
@@ -10594,7 +10594,7 @@
     </row>
     <row r="263" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A263" s="37">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="B263" s="35" t="s">
         <v>584</v>
@@ -10633,7 +10633,7 @@
       <c r="E264" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="T264" s="48" t="s">
+      <c r="T264" s="42" t="s">
         <v>589</v>
       </c>
     </row>
@@ -10656,7 +10656,7 @@
     </row>
     <row r="266" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A266" s="37">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B266" s="35" t="s">
         <v>586</v>
@@ -10681,7 +10681,7 @@
     </row>
     <row r="267" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A267" s="37">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B267" s="35" t="s">
         <v>586</v>
@@ -10706,7 +10706,7 @@
     </row>
     <row r="268" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A268" s="37">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B268" s="35" t="s">
         <v>586</v>
@@ -10731,7 +10731,7 @@
     </row>
     <row r="269" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A269" s="37">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B269" s="35" t="s">
         <v>586</v>
@@ -13056,31 +13056,31 @@
         <v>using-well-known</v>
       </c>
     </row>
-    <row r="374" spans="1:20" s="49" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A374" s="49">
+    <row r="374" spans="1:20" s="43" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A374" s="43">
         <v>373</v>
       </c>
-      <c r="B374" s="50" t="s">
+      <c r="B374" s="44" t="s">
         <v>605</v>
       </c>
-      <c r="C374" s="51" t="s">
+      <c r="C374" s="45" t="s">
         <v>606</v>
       </c>
-      <c r="D374" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="E374" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="M374" s="49" t="str" cm="1">
+      <c r="D374" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="E374" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="M374" s="43" t="str" cm="1">
         <f t="array" ref="M374">PAGE_NAME(B374)</f>
         <v>conformance</v>
       </c>
-      <c r="N374" s="49" t="str" cm="1">
+      <c r="N374" s="43" t="str" cm="1">
         <f t="array" ref="N374">SECTION_NAME(B374)</f>
         <v>using-well-known</v>
       </c>
-      <c r="T374" s="49" t="s">
+      <c r="T374" s="43" t="s">
         <v>607</v>
       </c>
     </row>
@@ -13315,31 +13315,31 @@
         <v>metadata</v>
       </c>
     </row>
-    <row r="384" spans="1:20" s="49" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A384" s="49">
+    <row r="384" spans="1:20" s="43" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A384" s="43">
         <v>383</v>
       </c>
-      <c r="B384" s="50" t="s">
+      <c r="B384" s="44" t="s">
         <v>609</v>
       </c>
-      <c r="C384" s="51" t="s">
+      <c r="C384" s="45" t="s">
         <v>608</v>
       </c>
-      <c r="D384" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="E384" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="M384" s="49" t="str" cm="1">
+      <c r="D384" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="E384" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="M384" s="43" t="str" cm="1">
         <f t="array" ref="M384">PAGE_NAME(B384)</f>
         <v>conformance</v>
       </c>
-      <c r="N384" s="49" t="str" cm="1">
+      <c r="N384" s="43" t="str" cm="1">
         <f t="array" ref="N384">SECTION_NAME(B384)</f>
         <v>metadata</v>
       </c>
-      <c r="T384" s="49" t="s">
+      <c r="T384" s="43" t="s">
         <v>591</v>
       </c>
     </row>
@@ -15604,14 +15604,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="409.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="52" t="s">
         <v>588</v>
       </c>
-      <c r="B1" s="47"/>
+      <c r="B1" s="52"/>
     </row>
     <row r="2" spans="1:3" ht="82.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
@@ -15829,19 +15829,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -15850,7 +15837,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC335ED7BB179244BF94A0DFE64544DC" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3a0f66abe5d2a0564332877ab55d3f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eebd8b74-b9de-41b2-9247-c010c4973c2b" xmlns:ns3="b7009bbd-f938-489b-a530-f05273710fff" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ec7ca2ee893ff8a0f61d4046c6461645" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
@@ -16104,25 +16091,20 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -16130,7 +16112,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E19681A-8DD3-40CB-9262-8533E89B98A6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16148,4 +16130,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>